<commit_message>
fix the import bug
</commit_message>
<xml_diff>
--- a/EasyRemoteDesktop/bin/Debug/服务器清单.xlsx
+++ b/EasyRemoteDesktop/bin/Debug/服务器清单.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>10.158.33.47</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -57,10 +57,6 @@
   <si>
     <t>账号密码</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>administrator/123456</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>administrator/123456</t>
@@ -75,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,15 +113,6 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -185,15 +172,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -210,13 +194,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,7 +477,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -518,11 +498,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -534,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -545,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -777,10 +757,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="administrator/@bcSmes!47"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>